<commit_message>
:white_check_mark: Escritas de teste
Correção de ISO e implementando o métod Gherkin
</commit_message>
<xml_diff>
--- a/Escritas em Normas Iso.29119-3/Gestão de teste_ iso.xlsx
+++ b/Escritas em Normas Iso.29119-3/Gestão de teste_ iso.xlsx
@@ -142,7 +142,7 @@
     <t>Com o "Site" aberto verificar se tem a proposta escrita em sua apresentação</t>
   </si>
   <si>
-    <t>A tela se adequa aquilo que foi apresentado</t>
+    <t>A tela se adequa aquilo que foi proposto</t>
   </si>
   <si>
     <t>A proposta está correta</t>
@@ -271,7 +271,7 @@
     <t>Deverá aparecer a palavra "Peso" no campo de inserção</t>
   </si>
   <si>
-    <t>A palavra "Peso" deverá aparecer</t>
+    <t>A palavra "Peso" deverá aparecer como indicador</t>
   </si>
   <si>
     <t>A palavra "Peso" aparece no campo de inserção de números</t>
@@ -283,10 +283,10 @@
     <t>O campo deverá ficar habilitado a escrita</t>
   </si>
   <si>
-    <t>Cursor de texto deverá ficar ativo e a palavra texto desaparecerá</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colocar o " Peso " igual a 85 e clicar em calcular </t>
+    <t>Cursor de texto deverá ficar ativo e a palavra "Peso" desaparecerá</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colocar o " Peso " igual a 85kg e clicar em calcular </t>
   </si>
   <si>
     <t>Obter valores de ml e litros de água</t>
@@ -381,7 +381,7 @@
     <t>Após calcular o valor inserido ainda continua no campo de inserção de números</t>
   </si>
   <si>
-    <t>Apagar o campor de inserção de números e não inserir nenhum valor</t>
+    <t>Apagar o campo de inserção de números e não inserir nenhum valor, clicando em calcular</t>
   </si>
   <si>
     <t>Irá aparecer a mensagem 'Insira um valor"</t>
@@ -390,7 +390,7 @@
     <t>Mensagem "O resultado é igual a 0 mL / 0 Litros"</t>
   </si>
   <si>
-    <t xml:space="preserve">Ao colocar o " Peso " em valor abaixo de 0 </t>
+    <t>Ao colocar o " Peso " em valor abaixo de 0 e clicar em calcular</t>
   </si>
   <si>
     <t>Irá aparecer a mensagem " O número não pode ser menor que 0 kg "</t>
@@ -399,7 +399,7 @@
     <t>Mensagem " O número não pode ser menor que 0 kg "</t>
   </si>
   <si>
-    <t>Ao colocar um valor grande como " 700 "kg</t>
+    <t>Ao colocar o " Peso " em valor  como " 700 "kg e clicar em calcular</t>
   </si>
   <si>
     <t>Irá aparecer a mensagem " O número não pode ser maior do que 700 kg "</t>
@@ -408,7 +408,7 @@
     <t>Não teve nenhuma ação</t>
   </si>
   <si>
-    <t xml:space="preserve">Colocar o " Peso " igual a 100 e clicar em calcular </t>
+    <t xml:space="preserve">Colocar o " Peso " igual a 100klg e clicar em calcular </t>
   </si>
   <si>
     <t>Mensagem na tela: O resultado é igual a 3500 mL / 3.5 Litros</t>

</xml_diff>